<commit_message>
Optimized the solution for 3d10.
</commit_message>
<xml_diff>
--- a/data/courses/3d/solutions/3d10.xlsx
+++ b/data/courses/3d/solutions/3d10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\home\nodchip\icfpc2024\data\courses\3d\solutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C610D7-7E51-4EFC-BD37-10237B303747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D0B361-8122-4594-9533-368E90001B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0F108AEB-1856-463D-8B1F-3B87ADA1D381}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0F108AEB-1856-463D-8B1F-3B87ADA1D381}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="29">
   <si>
     <t>.</t>
     <phoneticPr fontId="1"/>
@@ -122,10 +122,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>9</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>13</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -138,19 +134,23 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>17</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>-4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>-6</t>
+    <t>16</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>7</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>15</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-7</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-3</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -538,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4294CABA-F741-46C5-B90E-323E102FBDB4}">
-  <dimension ref="A1:AC23"/>
+  <dimension ref="A1:AA23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -551,7 +551,7 @@
     <col min="4" max="16384" width="3.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -633,14 +633,8 @@
       <c r="AA1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>0</v>
-      </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -722,14 +716,8 @@
       <c r="AA2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>0</v>
-      </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -811,14 +799,8 @@
       <c r="AA3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="1" t="s">
-        <v>0</v>
-      </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -880,7 +862,7 @@
         <v>0</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V4" s="1" t="s">
         <v>0</v>
@@ -900,14 +882,8 @@
       <c r="AA4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="1" t="s">
-        <v>0</v>
-      </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -966,13 +942,13 @@
         <v>0</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="W5" s="1" t="s">
         <v>0</v>
@@ -989,14 +965,8 @@
       <c r="AA5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="1" t="s">
-        <v>0</v>
-      </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -1078,14 +1048,8 @@
       <c r="AA6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="1" t="s">
-        <v>0</v>
-      </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -1135,22 +1099,22 @@
         <v>0</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="W7" s="1" t="s">
         <v>0</v>
@@ -1167,14 +1131,8 @@
       <c r="AA7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC7" s="1" t="s">
-        <v>0</v>
-      </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1221,16 +1179,16 @@
         <v>0</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="T8" s="1" t="s">
         <v>0</v>
@@ -1256,14 +1214,8 @@
       <c r="AA8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="1" t="s">
-        <v>0</v>
-      </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -1322,13 +1274,13 @@
         <v>0</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U9" s="1" t="s">
         <v>0</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="W9" s="1" t="s">
         <v>0</v>
@@ -1345,14 +1297,8 @@
       <c r="AA9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB9" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="1" t="s">
-        <v>0</v>
-      </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1402,13 +1348,13 @@
         <v>0</v>
       </c>
       <c r="Q10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S10" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="T10" s="1" t="s">
         <v>0</v>
@@ -1432,16 +1378,10 @@
         <v>0</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1500,13 +1440,13 @@
         <v>0</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="W11" s="1" t="s">
         <v>0</v>
@@ -1515,22 +1455,16 @@
         <v>0</v>
       </c>
       <c r="Y11" s="1" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="Z11" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AA11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -1580,7 +1514,7 @@
         <v>0</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="R12" s="1" t="s">
         <v>0</v>
@@ -1592,7 +1526,7 @@
         <v>0</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="V12" s="1" t="s">
         <v>0</v>
@@ -1604,22 +1538,16 @@
         <v>0</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z12" s="1" t="s">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="Z12" s="1">
+        <v>16</v>
       </c>
       <c r="AA12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AC12" s="1" t="s">
-        <v>0</v>
-      </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -1663,52 +1591,46 @@
         <v>0</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="R13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="U13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X13" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="S13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="T13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="U13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="V13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="W13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="X13" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="Y13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="Z13" s="1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AA13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC13" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1754,50 +1676,44 @@
       <c r="O14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="P14" s="1" t="s">
-        <v>0</v>
+      <c r="P14" s="1">
+        <v>16</v>
       </c>
       <c r="Q14" s="1" t="s">
         <v>0</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="T14" s="1" t="s">
         <v>0</v>
       </c>
       <c r="U14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X14" s="1">
         <v>16</v>
       </c>
-      <c r="V14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="W14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="X14" s="1" t="s">
-        <v>0</v>
-      </c>
       <c r="Y14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Z14" s="1">
-        <v>17</v>
+      <c r="Z14" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="AA14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC14" s="1" t="s">
-        <v>0</v>
-      </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -1847,31 +1763,31 @@
         <v>0</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="S15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="U15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="W15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="T15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="U15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="W15" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="X15" s="1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="Z15" s="1" t="s">
         <v>0</v>
@@ -1879,14 +1795,8 @@
       <c r="AA15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC15" s="1" t="s">
-        <v>0</v>
-      </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -1938,26 +1848,26 @@
       <c r="Q16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R16" s="1" t="s">
-        <v>0</v>
+      <c r="R16" s="1">
+        <v>16</v>
       </c>
       <c r="S16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="T16" s="1">
-        <v>17</v>
+      <c r="T16" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="U16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="V16" s="1" t="s">
-        <v>0</v>
+      <c r="V16" s="1">
+        <v>16</v>
       </c>
       <c r="W16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="X16" s="1">
-        <v>17</v>
+      <c r="X16" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="Y16" s="1" t="s">
         <v>0</v>
@@ -1968,14 +1878,8 @@
       <c r="AA16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AB16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC16" s="1" t="s">
-        <v>0</v>
-      </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -1989,527 +1893,491 @@
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T18" s="1">
+        <v>16</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M17" s="1" t="s">
+      <c r="F19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O17" s="1" t="s">
+      <c r="B20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="P17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="T17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="U17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="V17" s="1" t="s">
+      <c r="K21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="W17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="X17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC17" s="1" t="s">
+      <c r="E22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="R18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="T18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="U18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="V18" s="1">
-        <v>17</v>
-      </c>
-      <c r="W18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="X18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC18" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="T19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="U19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="V19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="W19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="X19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC19" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="T20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="U20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="V20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="W20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="X20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC20" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D21" s="1">
-        <v>17</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H21" s="1">
-        <v>17</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="T21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="U21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="V21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="W21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="X21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC21" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.4">
-      <c r="A22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="T22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="U22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="V22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="W22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="X22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC22" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -2520,13 +2388,13 @@
         <v>0</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F23" s="1">
-        <v>17</v>
+      <c r="F23" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>0</v>
@@ -2589,12 +2457,6 @@
         <v>0</v>
       </c>
       <c r="AA23" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB23" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC23" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>